<commit_message>
render table directly in html
</commit_message>
<xml_diff>
--- a/app/uploads/kirin_dataset.xlsx
+++ b/app/uploads/kirin_dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lawrence\Documents\GitHub\training-data-cleaner\app\test_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275C8AC2-B37B-4DC6-9C22-3A3CDACE7E06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1388CD58-A402-446A-B890-B35675C7163E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="training_data" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
   <si>
     <t>JA</t>
   </si>
@@ -278,6 +278,9 @@
   </si>
   <si>
     <t>giraffe</t>
+  </si>
+  <si>
+    <t>He lives in a flock&lt;br&gt;&lt;br&gt; of about 10-20, with a loose connection that fluctuates the composition and population.</t>
   </si>
 </sst>
 </file>
@@ -682,7 +685,7 @@
   <dimension ref="A1:B78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -751,7 +754,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>